<commit_message>
Corrected scale conversion bug from Double to Float
</commit_message>
<xml_diff>
--- a/test/test.xlsx
+++ b/test/test.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="72">
   <si>
     <t>HYPERION PART NUMBER:</t>
   </si>
@@ -164,13 +164,16 @@
     <t>17.15</t>
   </si>
   <si>
+    <t>20.00</t>
+  </si>
+  <si>
+    <t>19.85</t>
+  </si>
+  <si>
+    <t>20.15</t>
+  </si>
+  <si>
     <t>19.00</t>
-  </si>
-  <si>
-    <t>18.85</t>
-  </si>
-  <si>
-    <t>19.15</t>
   </si>
   <si>
     <t>21.00</t>
@@ -990,7 +993,7 @@
       </c>
     </row>
     <row r="68">
-      <c r="B68" t="n" s="2">
+      <c r="B68" t="n" s="3">
         <v>9.0</v>
       </c>
       <c r="C68" t="s" s="1">
@@ -1012,7 +1015,7 @@
         <v>52</v>
       </c>
       <c r="I68" t="s" s="1">
-        <v>50</v>
+        <v>53</v>
       </c>
     </row>
     <row r="69">
@@ -1023,7 +1026,7 @@
         <v>23</v>
       </c>
       <c r="D69" t="s" s="1">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="E69" t="s" s="1">
         <v>25</v>
@@ -1032,13 +1035,13 @@
         <v>26</v>
       </c>
       <c r="G69" t="s" s="1">
+        <v>55</v>
+      </c>
+      <c r="H69" t="s" s="1">
+        <v>56</v>
+      </c>
+      <c r="I69" t="s" s="1">
         <v>54</v>
-      </c>
-      <c r="H69" t="s" s="1">
-        <v>55</v>
-      </c>
-      <c r="I69" t="s" s="1">
-        <v>53</v>
       </c>
     </row>
     <row r="70">
@@ -1049,7 +1052,7 @@
         <v>23</v>
       </c>
       <c r="D70" t="s" s="1">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="E70" t="s" s="1">
         <v>25</v>
@@ -1058,13 +1061,13 @@
         <v>26</v>
       </c>
       <c r="G70" t="s" s="1">
+        <v>58</v>
+      </c>
+      <c r="H70" t="s" s="1">
+        <v>59</v>
+      </c>
+      <c r="I70" t="s" s="1">
         <v>57</v>
-      </c>
-      <c r="H70" t="s" s="1">
-        <v>58</v>
-      </c>
-      <c r="I70" t="s" s="1">
-        <v>56</v>
       </c>
     </row>
     <row r="71">
@@ -1075,7 +1078,7 @@
         <v>23</v>
       </c>
       <c r="D71" t="s" s="1">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="E71" t="s" s="1">
         <v>25</v>
@@ -1084,13 +1087,13 @@
         <v>26</v>
       </c>
       <c r="G71" t="s" s="1">
+        <v>61</v>
+      </c>
+      <c r="H71" t="s" s="1">
+        <v>62</v>
+      </c>
+      <c r="I71" t="s" s="1">
         <v>60</v>
-      </c>
-      <c r="H71" t="s" s="1">
-        <v>61</v>
-      </c>
-      <c r="I71" t="s" s="1">
-        <v>59</v>
       </c>
     </row>
     <row r="72">
@@ -1101,7 +1104,7 @@
         <v>23</v>
       </c>
       <c r="D72" t="s" s="1">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="E72" t="s" s="1">
         <v>25</v>
@@ -1110,13 +1113,13 @@
         <v>26</v>
       </c>
       <c r="G72" t="s" s="1">
+        <v>64</v>
+      </c>
+      <c r="H72" t="s" s="1">
+        <v>65</v>
+      </c>
+      <c r="I72" t="s" s="1">
         <v>63</v>
-      </c>
-      <c r="H72" t="s" s="1">
-        <v>64</v>
-      </c>
-      <c r="I72" t="s" s="1">
-        <v>62</v>
       </c>
     </row>
     <row r="73">
@@ -1127,7 +1130,7 @@
         <v>23</v>
       </c>
       <c r="D73" t="s" s="1">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="E73" t="s" s="1">
         <v>25</v>
@@ -1136,13 +1139,13 @@
         <v>26</v>
       </c>
       <c r="G73" t="s" s="1">
+        <v>67</v>
+      </c>
+      <c r="H73" t="s" s="1">
+        <v>68</v>
+      </c>
+      <c r="I73" t="s" s="1">
         <v>66</v>
-      </c>
-      <c r="H73" t="s" s="1">
-        <v>67</v>
-      </c>
-      <c r="I73" t="s" s="1">
-        <v>65</v>
       </c>
     </row>
     <row r="74">
@@ -1153,7 +1156,7 @@
         <v>23</v>
       </c>
       <c r="D74" t="s" s="1">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="E74" t="s" s="1">
         <v>25</v>
@@ -1162,13 +1165,13 @@
         <v>26</v>
       </c>
       <c r="G74" t="s" s="1">
+        <v>70</v>
+      </c>
+      <c r="H74" t="s" s="1">
+        <v>71</v>
+      </c>
+      <c r="I74" t="s" s="1">
         <v>69</v>
-      </c>
-      <c r="H74" t="s" s="1">
-        <v>70</v>
-      </c>
-      <c r="I74" t="s" s="1">
-        <v>68</v>
       </c>
     </row>
   </sheetData>

</xml_diff>